<commit_message>
updated excels and paper with scaled NMF expierments
</commit_message>
<xml_diff>
--- a/experiments/real_data/real_data.xlsx
+++ b/experiments/real_data/real_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkovacs/OneDrive - The Alan Turing Institute/OXFORD/DPhil_Mathematics_Oxford/Research/Code/Python/Pattern_Mining/column_generation/CG_new/experiments/real_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6B6D60-4B63-3B48-83EB-5212B4655695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88C8B5B-286F-6D4E-8279-06AA65EDD8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="19240" xr2:uid="{F644273B-ABDE-7943-991B-CE9773D43BD1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{F644273B-ABDE-7943-991B-CE9773D43BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="58">
   <si>
     <t>ASSO++</t>
   </si>
@@ -195,13 +195,34 @@
   </si>
   <si>
     <t>[0.7, 0.9]</t>
+  </si>
+  <si>
+    <t>threshold</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t>nndsvda</t>
+  </si>
+  <si>
+    <t>nndsvd</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>random seed</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,6 +241,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -272,6 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -281,7 +310,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +630,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +675,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -672,11 +703,10 @@
       <c r="H2" s="5">
         <v>367</v>
       </c>
-      <c r="I2" s="5">
-        <f>NMF!C2</f>
-        <v>295</v>
-      </c>
-      <c r="K2" s="8" t="s">
+      <c r="I2" s="12">
+        <v>281</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="L2" t="s">
@@ -694,13 +724,12 @@
         <f>'k-Greedy'!F2</f>
         <v>1352</v>
       </c>
-      <c r="P2" s="5">
-        <f>NMF_completion!B2</f>
-        <v>1792</v>
+      <c r="P2" s="12">
+        <v>1529</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -726,11 +755,10 @@
       <c r="H3" s="5">
         <v>1251</v>
       </c>
-      <c r="I3" s="5">
-        <f>NMF!D2</f>
-        <v>1273</v>
-      </c>
-      <c r="K3" s="8"/>
+      <c r="I3" s="13">
+        <v>1267</v>
+      </c>
+      <c r="K3" s="9"/>
       <c r="L3" t="s">
         <v>30</v>
       </c>
@@ -746,13 +774,12 @@
         <f>'k-Greedy'!G2</f>
         <v>1416</v>
       </c>
-      <c r="P3" s="5">
-        <f>NMF_completion!B3</f>
-        <v>1346</v>
+      <c r="P3" s="13">
+        <v>1304</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -778,11 +805,10 @@
       <c r="H4" s="5">
         <v>1352</v>
       </c>
-      <c r="I4" s="5">
-        <f>NMF!E2</f>
-        <v>1427</v>
-      </c>
-      <c r="K4" s="8"/>
+      <c r="I4" s="13">
+        <v>1272</v>
+      </c>
+      <c r="K4" s="9"/>
       <c r="L4" t="s">
         <v>31</v>
       </c>
@@ -798,13 +824,12 @@
         <f>'k-Greedy'!H2</f>
         <v>1419</v>
       </c>
-      <c r="P4" s="5">
-        <f>NMF_completion!B4</f>
-        <v>2361</v>
+      <c r="P4" s="13">
+        <v>1876</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -830,11 +855,10 @@
       <c r="H5" s="6">
         <v>778</v>
       </c>
-      <c r="I5" s="6">
-        <f>NMF!F2</f>
-        <v>820</v>
-      </c>
-      <c r="K5" s="9"/>
+      <c r="I5" s="14">
+        <v>808</v>
+      </c>
+      <c r="K5" s="10"/>
       <c r="L5" s="1" t="s">
         <v>32</v>
       </c>
@@ -850,13 +874,12 @@
         <f>'k-Greedy'!I2</f>
         <v>1246</v>
       </c>
-      <c r="P5" s="6">
-        <f>NMF_completion!B5</f>
+      <c r="P5" s="14">
         <v>1268</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -884,11 +907,10 @@
       <c r="H6" s="7">
         <v>354</v>
       </c>
-      <c r="I6" s="5">
-        <f>NMF!C3</f>
-        <v>135</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="I6" s="12">
+        <v>140</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="L6" t="s">
@@ -906,13 +928,12 @@
         <f>'k-Greedy'!F3</f>
         <v>1004</v>
       </c>
-      <c r="P6" s="5">
-        <f>NMF_completion!C2</f>
-        <v>1832</v>
+      <c r="P6" s="12">
+        <v>1229</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -938,11 +959,10 @@
       <c r="H7" s="5">
         <v>887</v>
       </c>
-      <c r="I7" s="5">
-        <f>NMF!D3</f>
-        <v>1190</v>
-      </c>
-      <c r="K7" s="8"/>
+      <c r="I7" s="13">
+        <v>782</v>
+      </c>
+      <c r="K7" s="9"/>
       <c r="L7" t="s">
         <v>30</v>
       </c>
@@ -958,13 +978,12 @@
         <f>'k-Greedy'!G3</f>
         <v>1238</v>
       </c>
-      <c r="P7" s="5">
-        <f>NMF_completion!C3</f>
-        <v>1618</v>
+      <c r="P7" s="13">
+        <v>1172</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -990,11 +1009,10 @@
       <c r="H8" s="5">
         <v>1484</v>
       </c>
-      <c r="I8" s="5">
-        <f>NMF!E3</f>
-        <v>1112</v>
-      </c>
-      <c r="K8" s="8"/>
+      <c r="I8" s="13">
+        <v>1103</v>
+      </c>
+      <c r="K8" s="9"/>
       <c r="L8" t="s">
         <v>31</v>
       </c>
@@ -1010,13 +1028,12 @@
         <f>'k-Greedy'!H3</f>
         <v>1094</v>
       </c>
-      <c r="P8" s="5">
-        <f>NMF_completion!C4</f>
-        <v>2361</v>
+      <c r="P8" s="13">
+        <v>1634</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1042,11 +1059,10 @@
       <c r="H9" s="6">
         <v>719</v>
       </c>
-      <c r="I9" s="6">
-        <f>NMF!F3</f>
-        <v>729</v>
-      </c>
-      <c r="K9" s="9"/>
+      <c r="I9" s="14">
+        <v>721</v>
+      </c>
+      <c r="K9" s="10"/>
       <c r="L9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1062,13 +1078,12 @@
         <f>'k-Greedy'!I3</f>
         <v>853</v>
       </c>
-      <c r="P9" s="6">
-        <f>NMF_completion!C5</f>
-        <v>2353</v>
+      <c r="P9" s="14">
+        <v>900</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1096,11 +1111,10 @@
       <c r="H10" s="7">
         <v>377</v>
       </c>
-      <c r="I10" s="5">
-        <f>NMF!C4</f>
-        <v>319</v>
-      </c>
-      <c r="K10" s="10" t="s">
+      <c r="I10" s="12">
+        <v>51</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>10</v>
       </c>
       <c r="L10" t="s">
@@ -1118,13 +1132,12 @@
         <f>'k-Greedy'!F4</f>
         <v>646</v>
       </c>
-      <c r="P10" s="5">
-        <f>NMF_completion!D2</f>
-        <v>1949</v>
+      <c r="P10" s="12">
+        <v>851</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -1150,11 +1163,10 @@
       <c r="H11" s="5">
         <v>694</v>
       </c>
-      <c r="I11" s="5">
-        <f>NMF!D4</f>
-        <v>896</v>
-      </c>
-      <c r="K11" s="8"/>
+      <c r="I11" s="13">
+        <v>450</v>
+      </c>
+      <c r="K11" s="9"/>
       <c r="L11" t="s">
         <v>30</v>
       </c>
@@ -1170,13 +1182,12 @@
         <f>'k-Greedy'!G4</f>
         <v>1056</v>
       </c>
-      <c r="P11" s="5">
-        <f>NMF_completion!D3</f>
-        <v>2159</v>
+      <c r="P11" s="13">
+        <v>1013</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -1202,11 +1213,10 @@
       <c r="H12" s="5">
         <v>1525</v>
       </c>
-      <c r="I12" s="5">
-        <f>NMF!E4</f>
-        <v>1102</v>
-      </c>
-      <c r="K12" s="8"/>
+      <c r="I12" s="13">
+        <v>821</v>
+      </c>
+      <c r="K12" s="9"/>
       <c r="L12" t="s">
         <v>31</v>
       </c>
@@ -1222,13 +1232,12 @@
         <f>'k-Greedy'!H4</f>
         <v>881</v>
       </c>
-      <c r="P12" s="5">
-        <f>NMF_completion!D4</f>
-        <v>2361</v>
+      <c r="P12" s="13">
+        <v>1580</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1254,11 +1263,10 @@
       <c r="H13" s="6">
         <v>661</v>
       </c>
-      <c r="I13" s="6">
-        <f>NMF!F4</f>
-        <v>660</v>
-      </c>
-      <c r="K13" s="9"/>
+      <c r="I13" s="14">
+        <v>617</v>
+      </c>
+      <c r="K13" s="10"/>
       <c r="L13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1274,9 +1282,8 @@
         <f>'k-Greedy'!I4</f>
         <v>706</v>
       </c>
-      <c r="P13" s="6">
-        <f>NMF_completion!D5</f>
-        <v>3189</v>
+      <c r="P13" s="14">
+        <v>815</v>
       </c>
     </row>
   </sheetData>
@@ -1315,16 +1322,16 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1347,16 +1354,16 @@
       <c r="F2">
         <v>776</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="8">
         <v>1353</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="8">
         <v>1264</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="8">
         <v>1419</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="8">
         <v>1246</v>
       </c>
     </row>
@@ -1379,16 +1386,16 @@
       <c r="F3">
         <v>19.71649485</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="8">
         <v>0.88691796000000001</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="8">
         <v>19.620253200000001</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="8">
         <v>29.880197299999999</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1411,16 +1418,16 @@
       <c r="F4">
         <v>4.2027950000000001E-2</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <v>1.1897740400000001</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="8">
         <v>2.0839679200000001</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="8">
         <v>1.6400980999999999</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>0.29892587999999998</v>
       </c>
     </row>
@@ -1443,16 +1450,16 @@
       <c r="F5">
         <v>776</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="8">
         <v>1352</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="8">
         <v>1264</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="8">
         <v>1419</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="8">
         <v>1246</v>
       </c>
     </row>
@@ -1475,16 +1482,16 @@
       <c r="F6">
         <v>685</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="8">
         <v>963</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="8">
         <v>1176</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="8">
         <v>1064</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="8">
         <v>782</v>
       </c>
     </row>
@@ -1507,16 +1514,16 @@
       <c r="F7">
         <v>73.722627739999993</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>45.067497400000001</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="8">
         <v>100</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="8">
         <v>75.845864700000007</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="8">
         <v>14.1943734</v>
       </c>
     </row>
@@ -1539,16 +1546,16 @@
       <c r="F8">
         <v>0.131505013</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="8">
         <v>6.9059619899999998</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="8">
         <v>603.49428999999998</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="8">
         <v>10.910437099999999</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="8">
         <v>95.153837699999997</v>
       </c>
     </row>
@@ -1571,16 +1578,16 @@
       <c r="F9">
         <v>684</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>962</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="8">
         <v>1138</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="8">
         <v>1064</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="8">
         <v>779</v>
       </c>
     </row>
@@ -1603,16 +1610,16 @@
       <c r="F10">
         <v>578</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="8">
         <v>514</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="8">
         <v>950</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="8">
         <v>766</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <v>240</v>
       </c>
     </row>
@@ -1635,16 +1642,16 @@
       <c r="F11">
         <v>100</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="8">
         <v>100</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="8">
         <v>100</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="8">
         <v>100</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="8">
         <v>25.8333333</v>
       </c>
     </row>
@@ -1667,16 +1674,16 @@
       <c r="F12">
         <v>0.151741982</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="8">
         <v>1.18043184</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="8">
         <v>603.75460899999996</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="8">
         <v>6.7230849299999997</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <v>24.078275000000001</v>
       </c>
     </row>
@@ -1699,16 +1706,16 @@
       <c r="F13">
         <v>573</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="8">
         <v>514</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="8">
         <v>907</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="8">
         <v>765</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="8">
         <v>240</v>
       </c>
     </row>
@@ -2901,10 +2908,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4801727-B8C1-E84C-BCF4-E842CA30443C}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2931,16 +2938,16 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="D2">
-        <v>1273</v>
+        <v>1267</v>
       </c>
       <c r="E2">
-        <v>1427</v>
+        <v>1272</v>
       </c>
       <c r="F2">
-        <v>820</v>
+        <v>808</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2951,16 +2958,16 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D3">
-        <v>1190</v>
+        <v>782</v>
       </c>
       <c r="E3">
-        <v>1112</v>
+        <v>1103</v>
       </c>
       <c r="F3">
-        <v>729</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2971,16 +2978,16 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>319</v>
+        <v>51</v>
       </c>
       <c r="D4">
-        <v>896</v>
+        <v>450</v>
       </c>
       <c r="E4">
-        <v>1102</v>
+        <v>821</v>
       </c>
       <c r="F4">
-        <v>660</v>
+        <v>617</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2991,16 +2998,16 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>1.7809867858886699E-3</v>
+        <v>3.2670500000000001E-3</v>
       </c>
       <c r="D5">
-        <v>1.4410018920898401E-3</v>
+        <v>4.3988229999999996E-3</v>
       </c>
       <c r="E5">
-        <v>3.6768913269042899E-3</v>
+        <v>6.6189769999999998E-3</v>
       </c>
       <c r="F5">
-        <v>6.4706802368163997E-4</v>
+        <v>1.842022E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3011,16 +3018,16 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>6.0338973999023403E-3</v>
+        <v>2.2208689999999999E-3</v>
       </c>
       <c r="D6">
-        <v>3.9441585540771398E-3</v>
+        <v>5.6350230000000003E-3</v>
       </c>
       <c r="E6">
-        <v>6.7601203918456997E-3</v>
+        <v>9.812355E-3</v>
       </c>
       <c r="F6">
-        <v>4.8320293426513602E-3</v>
+        <v>6.3238139999999997E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3031,16 +3038,136 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>6.4730644226074201E-3</v>
+        <v>6.865978E-3</v>
       </c>
       <c r="D7">
-        <v>1.31127834320068E-2</v>
+        <v>6.7610739999999997E-3</v>
       </c>
       <c r="E7">
-        <v>1.17111206054687E-2</v>
+        <v>1.2351750999999999E-2</v>
       </c>
       <c r="F7">
-        <v>7.5669288635253898E-3</v>
+        <v>1.2714863E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+      <c r="F8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0.4</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+      <c r="F9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.4</v>
+      </c>
+      <c r="D10">
+        <v>0.4</v>
+      </c>
+      <c r="E10">
+        <v>0.5</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3050,79 +3177,183 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA93F51-6B5C-F642-9076-361C87C79515}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="D1">
+      <c r="D2">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B2">
-        <v>1792</v>
-      </c>
-      <c r="C2">
-        <v>1832</v>
-      </c>
-      <c r="D2">
-        <v>1949</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>1529</v>
+      </c>
+      <c r="C3">
+        <v>1229</v>
+      </c>
+      <c r="D3">
+        <v>851</v>
+      </c>
+      <c r="E3">
+        <v>0.7</v>
+      </c>
+      <c r="F3">
+        <v>0.6</v>
+      </c>
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B3">
-        <v>1346</v>
-      </c>
-      <c r="C3">
-        <v>1618</v>
-      </c>
-      <c r="D3">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>1304</v>
+      </c>
+      <c r="C4">
+        <v>1172</v>
+      </c>
+      <c r="D4">
+        <v>1013</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>0.4</v>
+      </c>
+      <c r="G4">
+        <v>0.4</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B4">
-        <v>2361</v>
-      </c>
-      <c r="C4">
-        <v>2361</v>
-      </c>
-      <c r="D4">
-        <v>2361</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>1876</v>
+      </c>
+      <c r="C5">
+        <v>1634</v>
+      </c>
+      <c r="D5">
+        <v>1580</v>
+      </c>
+      <c r="E5">
+        <v>0.8</v>
+      </c>
+      <c r="F5">
+        <v>0.9</v>
+      </c>
+      <c r="G5">
+        <v>0.8</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>1268</v>
       </c>
-      <c r="C5">
-        <v>2353</v>
-      </c>
-      <c r="D5">
-        <v>3189</v>
+      <c r="C6">
+        <v>900</v>
+      </c>
+      <c r="D6">
+        <v>815</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="F6">
+        <v>0.4</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>